<commit_message>
Time update, WIP of research journal added,.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-16may2016.xlsx
+++ b/time-labor/week-of-16may2016.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -355,7 +356,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -385,7 +386,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="10" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -393,7 +394,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="10" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -405,10 +406,6 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -488,16 +485,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -594,17 +583,17 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.02551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.88775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -697,8 +686,8 @@
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -706,15 +695,15 @@
         <v>8</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -722,15 +711,15 @@
         <v>10</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -738,15 +727,15 @@
         <v>12</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -754,8 +743,8 @@
         <v>14</v>
       </c>
       <c r="I10" s="7"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0"/>
@@ -770,254 +759,256 @@
       <c r="K11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22" t="n">
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21" t="n">
         <f aca="false">IF((((D13-C13)+(F13-E13))*24)&gt;8,8,((D13-C13)+(F13-E13))*24)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="22" t="n">
+      <c r="H13" s="21" t="n">
         <f aca="false">IF(((D13-C13)+(F13-E13))*24&gt;8,((D13-C13)+(F13-E13))*24-8,0)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="20" t="n">
+      <c r="C14" s="19" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="D14" s="21" t="n">
+      <c r="D14" s="20" t="n">
         <v>0.75</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22" t="n">
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21" t="n">
         <f aca="false">IF((((D14-C14)+(F14-E14))*24)&gt;8,8,((D14-C14)+(F14-E14))*24)</f>
         <v>5</v>
       </c>
-      <c r="H14" s="22" t="n">
+      <c r="H14" s="21" t="n">
         <f aca="false">IF(((D14-C14)+(F14-E14))*24&gt;8,((D14-C14)+(F14-E14))*24-8,0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="20" t="n">
+      <c r="C15" s="19" t="n">
         <v>0.5</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22" t="n">
+      <c r="D15" s="20" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21" t="n">
         <f aca="false">IF((((D15-C15)+(F15-E15))*24)&gt;8,8,((D15-C15)+(F15-E15))*24)</f>
-        <v>-12</v>
-      </c>
-      <c r="H15" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" s="21" t="n">
         <f aca="false">IF(((D15-C15)+(F15-E15))*24&gt;8,((D15-C15)+(F15-E15))*24-8,0)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22" t="n">
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21" t="n">
         <f aca="false">IF((((D16-C16)+(F16-E16))*24)&gt;8,8,((D16-C16)+(F16-E16))*24)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="22" t="n">
+      <c r="H16" s="21" t="n">
         <f aca="false">IF(((D16-C16)+(F16-E16))*24&gt;8,((D16-C16)+(F16-E16))*24-8,0)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="25"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22" t="n">
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="22" t="n">
+      <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="25"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22" t="n">
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21" t="n">
         <f aca="false">IF((((D18-C18)+(F18-E18))*24)&gt;8,8,((D18-C18)+(F18-E18))*24)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="22" t="n">
+      <c r="H18" s="21" t="n">
         <f aca="false">IF(((D18-C18)+(F18-E18))*24&gt;8,((D18-C18)+(F18-E18))*24-8,0)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="25"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22" t="n">
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21" t="n">
         <f aca="false">IF((((D19-C19)+(F19-E19))*24)&gt;8,8,((D19-C19)+(F19-E19))*24)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="22" t="n">
+      <c r="H19" s="21" t="n">
         <f aca="false">IF(((D19-C19)+(F19-E19))*24&gt;8,((D19-C19)+(F19-E19))*24-8,0)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="25"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="19" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="22" t="n">
+      <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>-7</v>
-      </c>
-      <c r="H20" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="22" t="n">
+      <c r="I20" s="21" t="n">
         <f aca="false">SUM(I13:I19)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="22" t="n">
+      <c r="J20" s="21" t="n">
         <f aca="false">SUM(J13:J19)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="25"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="19" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="29" t="n">
+      <c r="G21" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="H21" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="30"/>
+      <c r="H21" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="19" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="31" t="n">
+      <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>-70</v>
-      </c>
-      <c r="H22" s="31" t="n">
+        <v>100</v>
+      </c>
+      <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
         <v>0</v>
       </c>
-      <c r="I22" s="31" t="n">
+      <c r="I22" s="30" t="n">
         <f aca="false">I20*I21</f>
         <v>0</v>
       </c>
-      <c r="J22" s="31" t="n">
+      <c r="J22" s="30" t="n">
         <f aca="false">J20*J21</f>
         <v>0</v>
       </c>
-      <c r="K22" s="31" t="n">
+      <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>-70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1033,46 +1024,46 @@
       <c r="K23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="35"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="38" t="s">
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="35"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="38" t="s">
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="35" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>